<commit_message>
Enhanced button clicking with multiple methods and pointer events
</commit_message>
<xml_diff>
--- a/Br.net login .xlsx
+++ b/Br.net login .xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\smart\OneDrive\Desktop\Chatgpt1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B46AA36-07DD-42EF-AB6F-BD98D12BBE54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6080D1EA-AC64-4073-9A12-C8D4D83957D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{26A5588D-6DB4-4F1A-9805-B9C41FC223AD}"/>
   </bookViews>
@@ -721,7 +721,7 @@
   <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Update assistant code and clean up documentation files
</commit_message>
<xml_diff>
--- a/Br.net login .xlsx
+++ b/Br.net login .xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\smart\OneDrive\Desktop\Chatgpt1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04FEFD71-C8A7-46A8-B388-F24AA0CEC138}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF81B82A-F1DA-4FDF-9DE8-62A0B5AA272F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{26A5588D-6DB4-4F1A-9805-B9C41FC223AD}"/>
+    <workbookView minimized="1" xWindow="5988" yWindow="4404" windowWidth="17280" windowHeight="8880" xr2:uid="{26A5588D-6DB4-4F1A-9805-B9C41FC223AD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -724,7 +724,7 @@
   <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1080,8 +1080,9 @@
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="J4" r:id="rId1" xr:uid="{947F0E4E-8141-455A-A177-9AFCC71AB8A0}"/>
+    <hyperlink ref="I2" r:id="rId2" xr:uid="{D7DEEF10-34B3-4E03-8AA3-9CCE8A67F2E1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>